<commit_message>
added recipe Omurice met tofu
</commit_message>
<xml_diff>
--- a/Excel_files/data.xlsx
+++ b/Excel_files/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elskn\Projects\Grocery_list\Excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F46BC5-4B2F-4C6A-83F6-45880DFFCB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20AA309-95A9-4B79-AAE7-745919D55B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10158" yWindow="270" windowWidth="12498" windowHeight="11802" activeTab="1" xr2:uid="{F538357A-919F-47F2-8670-73C1BC41B637}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F538357A-919F-47F2-8670-73C1BC41B637}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="222">
   <si>
     <t>recipe_name</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>https://www.collectandgo.be/colruyt/nl/assortiment/everyday-fijn-keukenzout-1kg</t>
+  </si>
+  <si>
+    <t>Omurice met Tofu</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5913751C-1BC7-493E-BB20-B30D7F548B56}">
   <dimension ref="A1:D1029"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2564,69 +2567,212 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C107" s="2"/>
+      <c r="A107" t="s">
+        <v>221</v>
+      </c>
+      <c r="B107" t="s">
+        <v>71</v>
+      </c>
+      <c r="C107" s="2">
+        <v>64</v>
+      </c>
+      <c r="D107" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C108" s="2"/>
+      <c r="A108" t="s">
+        <v>221</v>
+      </c>
+      <c r="B108" t="s">
+        <v>49</v>
+      </c>
+      <c r="C108" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D108" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C109" s="2"/>
+      <c r="A109" t="s">
+        <v>221</v>
+      </c>
+      <c r="B109" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="D109" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C110" s="2"/>
+      <c r="A110" t="s">
+        <v>221</v>
+      </c>
+      <c r="B110" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D110" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C111" s="2"/>
+      <c r="A111" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" t="s">
+        <v>108</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D111" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C113" s="2"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C114" s="2"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C115" s="2"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C116" s="2"/>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C117" s="2"/>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C118" s="2"/>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C119" s="2"/>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" t="s">
+        <v>109</v>
+      </c>
+      <c r="C112" s="2">
+        <v>50</v>
+      </c>
+      <c r="D112" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>221</v>
+      </c>
+      <c r="B113" t="s">
+        <v>138</v>
+      </c>
+      <c r="C113" s="2">
+        <v>10</v>
+      </c>
+      <c r="D113" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" t="s">
+        <v>18</v>
+      </c>
+      <c r="C114" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="D114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
+        <v>221</v>
+      </c>
+      <c r="B115" t="s">
+        <v>93</v>
+      </c>
+      <c r="C115" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="D115" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" t="s">
+        <v>94</v>
+      </c>
+      <c r="C116" s="2">
+        <v>10</v>
+      </c>
+      <c r="D116" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="s">
+        <v>221</v>
+      </c>
+      <c r="B117" t="s">
+        <v>112</v>
+      </c>
+      <c r="C117" s="2">
+        <v>30</v>
+      </c>
+      <c r="D117" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" t="s">
+        <v>221</v>
+      </c>
+      <c r="B118" t="s">
+        <v>113</v>
+      </c>
+      <c r="C118" s="2">
+        <v>3</v>
+      </c>
+      <c r="D118" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" t="s">
+        <v>221</v>
+      </c>
+      <c r="B119" t="s">
+        <v>89</v>
+      </c>
+      <c r="C119" s="2">
+        <v>100</v>
+      </c>
+      <c r="D119" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C120" s="2"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" s="2"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C128" s="2"/>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.55000000000000004">
@@ -5352,7 +5498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD61BB9-6DAA-4988-9059-527D17889229}">
   <dimension ref="A1:G319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>

</xml_diff>